<commit_message>
Final risks and issues, plus activity diagram for section 2
</commit_message>
<xml_diff>
--- a/RAG Assessment CD.xlsx
+++ b/RAG Assessment CD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive - Durham University\Desktop\CS Level 2\Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\OneDrive - Durham University\Desktop\CS Level 2\Software Engineering\software-engineering-group-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8408FCB-2140-47B5-A580-5EB22FF9A067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0C5812-DBB2-419A-8AD7-9F6983DE4828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D6C8B683-8327-4F45-9493-C77DA598D25D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Capstone</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Reason</t>
-  </si>
-  <si>
     <t>RAG</t>
   </si>
   <si>
@@ -62,18 +59,12 @@
     <t>Green</t>
   </si>
   <si>
-    <t>I'm currently beginning an AI module and this would build on how it is particularly used in business.</t>
-  </si>
-  <si>
     <t>Getting Started with Enterprise Data Science</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/capstone?ach_id=8d72f699-26ac-4542-a701-6b69f50e6b5f</t>
   </si>
   <si>
-    <t>Data Science is currently a module in my course and so the course would build on that knowledge.</t>
-  </si>
-  <si>
     <t>https://www.ibm.com/academic/topic/capstone?ach_id=3f13c64c-c7ca-45d8-bce1-f05711460f09</t>
   </si>
   <si>
@@ -86,12 +77,6 @@
     <t>https://www.ibm.com/academic/topic/capstone?ach_id=b9de26db-b689-4894-bcad-5aa28deec936</t>
   </si>
   <si>
-    <t xml:space="preserve">Cybersecurity is a necessary part of Computer Science and as such relevant to my course. </t>
-  </si>
-  <si>
-    <t>Cloud computing is widely used across many industries, and I would be glad to work on a cloud-based software platform.</t>
-  </si>
-  <si>
     <t>Artificial Intelligence</t>
   </si>
   <si>
@@ -101,9 +86,6 @@
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=c7124e68-cce6-4dc4-b968-d65ba035a59f</t>
   </si>
   <si>
-    <t>It is likely to overlap with the Artificial Intelligence module.</t>
-  </si>
-  <si>
     <t>Fundamentals of Sustainability and Technology</t>
   </si>
   <si>
@@ -113,63 +95,42 @@
     <t>Amber</t>
   </si>
   <si>
-    <t>The course is of personal interest and likely to be useful to consider throughout my career.</t>
-  </si>
-  <si>
     <t>Building Trustworthy AI Enterprise Solutions</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=a0c78296-18d1-4e92-bebe-d31add4862e8</t>
   </si>
   <si>
-    <t>The course would help with group work in university. The course would also help prepare for the use of AI in the industry.</t>
-  </si>
-  <si>
     <t>Building AI Solutions Using Advanced Algorithms and Open Source Frameworks</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=d92c9dca-c230-4dfb-b214-d18c56104d5d</t>
   </si>
   <si>
-    <t xml:space="preserve">We have learned extensively about algorithms and slightly about neural networks, so the course would be adding to current knowledge. </t>
-  </si>
-  <si>
     <t>Art of Prompt Writing</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=9c047ace-65b8-4719-ba47-a6a9f0ffd975</t>
   </si>
   <si>
-    <t>The course would add a practical understanding of AI, which may also assist with our AI module.</t>
-  </si>
-  <si>
     <t>OpenDS4All</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=7de402f8-db6b-47a1-ad6c-d5ba028f7d2c</t>
   </si>
   <si>
-    <t>The github repository gives additional material which woulkd help with our current Data Science module.</t>
-  </si>
-  <si>
     <t>IBM AI Education</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=6d92def9-70bd-4307-9fe8-d2b7372b94f1</t>
   </si>
   <si>
-    <t>The course may be more helpful for educators, but it will also give students an idea of what is important about AI for the workforce.</t>
-  </si>
-  <si>
     <t>Watson Academy</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=dd44379d-d2c6-43ee-aba1-6f362052c2cb</t>
   </si>
   <si>
-    <t>Although the course may give some general ideas about AI, learning about Watson may be too specialised for students.</t>
-  </si>
-  <si>
     <t>Data Refinery Essentials</t>
   </si>
   <si>
@@ -179,27 +140,18 @@
     <t>Red</t>
   </si>
   <si>
-    <t>Data Refinery is unlikely to be directly used in university work, but may be useful for external projects.</t>
-  </si>
-  <si>
     <t>IBM Watson Knowledge Catalog Essentials</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=4eb246ce-2c42-485e-a50a-47815da40831</t>
   </si>
   <si>
-    <t>Students are unlikely to need to catalogue such large amounts of data for university work.</t>
-  </si>
-  <si>
     <t>Create a Node-RED starter application</t>
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/artificial-intelligence?ach_id=6ba25c43-1f7f-4762-8924-3dd71d5e3c08</t>
   </si>
   <si>
-    <t>Learning to build a Node-RED application may not be helpful for university, it is helpful for quickly building applications.</t>
-  </si>
-  <si>
     <t>Data Science</t>
   </si>
   <si>
@@ -207,6 +159,78 @@
   </si>
   <si>
     <t>https://www.ibm.com/academic/topic/data-science?ach_id=9cd4e0d9-5c96-4866-9b29-c76e511e22b7</t>
+  </si>
+  <si>
+    <t>Machine Learning for Data Science Projects</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=2bdf0308-8170-455d-8936-9a036ea290a3</t>
+  </si>
+  <si>
+    <t>Data Fundamentals</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=e5c3f98b-ee96-45d4-b153-d58b1efb8b30</t>
+  </si>
+  <si>
+    <t>Constraint Programming with ILOG CP Optimizer</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=520052ab-1ee5-48c5-8f8f-a614a0971bb5</t>
+  </si>
+  <si>
+    <t>Overview of IBM Cognos Analytics</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=fcce46b0-df00-4abc-9b02-cefc3c52ef08</t>
+  </si>
+  <si>
+    <t>IBM Planning Analytics - Design and Develop Models in Planning Analytics Workspace</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=94366672-0dd3-4ac6-bf44-9a0d78c43926</t>
+  </si>
+  <si>
+    <t>IBM Planning Analytics - Analyze Data and Create Reports</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=202b1758-c742-45c3-a8d2-d227bc01c6b8</t>
+  </si>
+  <si>
+    <t>IBM Cognos Framework Manager - Design Metadata Models</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=c6009472-5471-4d40-a3d4-c68fde05ceb4</t>
+  </si>
+  <si>
+    <t>IBM Cognos Analytics - Author Reports Fundamentals</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=72ba50d6-da72-407e-a8f8-1a0c1e3c972f</t>
+  </si>
+  <si>
+    <t>IBM Cognos Analytics - Author Reports Advanced</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=31fea6d3-db52-4277-9a4d-0dc964f41c80</t>
+  </si>
+  <si>
+    <t>IBM Cognos Analytics - Author Reports with Multidimensional Data</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=0fd39d43-923f-4c81-9d04-3eb642192833</t>
+  </si>
+  <si>
+    <t>IBM Cognos Analytics - Architecture and Logging</t>
+  </si>
+  <si>
+    <t>https://www.ibm.com/academic/topic/data-science?ach_id=cb5cf932-60fd-4bbd-9951-1bc8c0900e78</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>IBM Automation Learning Center</t>
   </si>
 </sst>
 </file>
@@ -274,10 +298,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -312,18 +333,13 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E3334F9-BF8D-4B50-8CAC-1B728E393712}" name="Table1" displayName="Table1" ref="A3:E46" headerRowCount="0" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="5">
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BF552041-B1B2-4235-8AAB-6960EAD657DC}" name="Capstone" totalsRowLabel="Total" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{61D358E7-B46B-42CC-8A8C-C2D979C6E9CA}" name="Name" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{A9717A9D-9B6C-445A-AF0E-E3C51BDF89C2}" name="Column3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{01206309-1FC4-48B3-9E1D-5D1EDF5E0E5A}" name="Column4" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{93BDEAF5-5F5B-4C70-AAC7-AE1FB11FB42D}" name="Column5" totalsRowFunction="count" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2E3334F9-BF8D-4B50-8CAC-1B728E393712}" name="Table1" displayName="Table1" ref="A3:D46" headerRowCount="0" headerRowDxfId="6" dataDxfId="5" totalsRowDxfId="4">
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{BF552041-B1B2-4235-8AAB-6960EAD657DC}" name="Capstone" totalsRowLabel="Total" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{61D358E7-B46B-42CC-8A8C-C2D979C6E9CA}" name="Name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{A9717A9D-9B6C-445A-AF0E-E3C51BDF89C2}" name="Column3" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{01206309-1FC4-48B3-9E1D-5D1EDF5E0E5A}" name="Column4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -626,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7A2D04-D5B0-4A2A-86F0-6412B3C99510}">
-  <dimension ref="A3:E46"/>
+  <dimension ref="A3:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -637,7 +653,7 @@
     <col min="1" max="5" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,466 +661,479 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="B34" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C14" r:id="rId1" xr:uid="{F116257C-A062-49E9-94D0-A7817922C70B}"/>
     <hyperlink ref="C15" r:id="rId2" xr:uid="{7E56C67E-35B0-4277-8047-678416D19A9B}"/>
     <hyperlink ref="C19" r:id="rId3" xr:uid="{1DDC6FD6-5B0C-46D9-9286-7D4EEFF31FBA}"/>
+    <hyperlink ref="C25" r:id="rId4" xr:uid="{59829C36-1EBC-4680-BBFB-958EB7DFB4FC}"/>
+    <hyperlink ref="C27" r:id="rId5" xr:uid="{7F14205D-C5A3-46D9-9A9D-8F2B763F7E20}"/>
+    <hyperlink ref="C28" r:id="rId6" xr:uid="{0EBDAB8D-0611-4E3F-A0A4-11CC6790EC33}"/>
+    <hyperlink ref="C29" r:id="rId7" xr:uid="{EFD6DAFB-E41C-44C7-BDBD-DC4C07B77FBA}"/>
+    <hyperlink ref="C30" r:id="rId8" xr:uid="{00563540-2280-4382-8A3A-045EB23AB1D4}"/>
+    <hyperlink ref="C31" r:id="rId9" xr:uid="{7DF0F570-1CE4-4010-A7DB-D785F6264D09}"/>
+    <hyperlink ref="C32" r:id="rId10" xr:uid="{D7545B4D-66EC-4FC5-90F0-B4DC6C601CB2}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{B1E2CF6D-4314-400A-AC71-D896779423AD}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{9013DC54-9EE7-4D45-9D9F-A3B2C390A767}"/>
+    <hyperlink ref="C16" r:id="rId13" xr:uid="{82BF736D-5778-42F3-9EC9-DB2CB53C5FFB}"/>
+    <hyperlink ref="C17" r:id="rId14" xr:uid="{8FC9A41D-01BE-44D0-AB8D-B9C09DC39D36}"/>
+    <hyperlink ref="C18" r:id="rId15" xr:uid="{035AB7BF-08E9-45EF-B292-429BDCBEF537}"/>
+    <hyperlink ref="C5" r:id="rId16" xr:uid="{AD6AF2C6-27FB-43CC-AC34-563CF88E5726}"/>
+    <hyperlink ref="C21" r:id="rId17" xr:uid="{7414E392-1C28-4D7C-9F8D-64439A1F1DD1}"/>
+    <hyperlink ref="C22" r:id="rId18" xr:uid="{F8BACE90-0890-44CE-8937-A86E6F81AA7D}"/>
+    <hyperlink ref="C23" r:id="rId19" xr:uid="{ACEDBFCF-C523-43C4-B6E0-31434D59A6DE}"/>
+    <hyperlink ref="C24" r:id="rId20" xr:uid="{799F3B86-8533-4671-B33F-DC4408DCBB9F}"/>
+    <hyperlink ref="C26" r:id="rId21" xr:uid="{A1A16CC8-E935-4DDA-8638-7C7DBC4F89B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5cbbcd18-735e-4945-9551-c599062a39c3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1335,27 +1364,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5cbbcd18-735e-4945-9551-c599062a39c3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FF94E9E-1D96-4673-974C-E2ACDAABD363}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22062B4A-BE1A-4A0E-B2D6-3F29ACAC54C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fad2bf6-c688-432e-8b8e-5df8ea12fc2c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5cbbcd18-735e-4945-9551-c599062a39c3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1380,9 +1399,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22062B4A-BE1A-4A0E-B2D6-3F29ACAC54C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FF94E9E-1D96-4673-974C-E2ACDAABD363}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fad2bf6-c688-432e-8b8e-5df8ea12fc2c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5cbbcd18-735e-4945-9551-c599062a39c3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>